<commit_message>
Still working on it
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14175" windowHeight="5745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14175" windowHeight="5745" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
+    <sheet name="Calc Report" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="13">
   <si>
     <r>
       <t>X</t>
@@ -1452,11 +1453,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="292642672"/>
-        <c:axId val="292643232"/>
+        <c:axId val="218988512"/>
+        <c:axId val="218989072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="292642672"/>
+        <c:axId val="218988512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1562,12 +1563,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292643232"/>
+        <c:crossAx val="218989072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="292643232"/>
+        <c:axId val="218989072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1697,7 +1698,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292642672"/>
+        <c:crossAx val="218988512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2461,11 +2462,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="394948560"/>
-        <c:axId val="394949120"/>
+        <c:axId val="292721760"/>
+        <c:axId val="292722320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="394948560"/>
+        <c:axId val="292721760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2571,12 +2572,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="394949120"/>
+        <c:crossAx val="292722320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="394949120"/>
+        <c:axId val="292722320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2706,7 +2707,1702 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="394948560"/>
+        <c:crossAx val="292721760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.33581529723114828"/>
+          <c:y val="0.90914035525057801"/>
+          <c:w val="0.40328916814524313"/>
+          <c:h val="4.1705562395755076E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Equilibrium Concentration of Carbon in Various Environments</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Tropical</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'Calc Report'!$A$11:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>X1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>X2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>X3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>X4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>X7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calc Report'!$B$11:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1540</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7000.9999999999991</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1540</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>616</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10011.000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Grass</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'Calc Report'!$A$11:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>X1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>X2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>X3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>X4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>X7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calc Report'!$C$11:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>683</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17302</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10814</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Agricultural</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'Calc Report'!$A$11:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>X1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>X2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>X3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>X4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>X7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calc Report'!$D$11:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>345.00000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>345.00000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3879</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3879</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="300460656"/>
+        <c:axId val="300461216"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="300460656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Ecosystem Components X</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="-25000"/>
+                  <a:t>i</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>, i=1, 2, ... ,7</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="300461216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="300461216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="89000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="0"/>
+                      <a:lumOff val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="0"/>
+                      <a:lumOff val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="16000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="2700000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Grams of Carbon Per Square Meter</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="300460656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.33581529723114828"/>
+          <c:y val="0.90914035525057801"/>
+          <c:w val="0.20092187705175873"/>
+          <c:h val="4.1705562395755076E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Time Needed</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> For Carbon </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Concentration to Reach 95% of its Stable Value in Various Components of the Ecosystem &amp; Various Ecosystems</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calc Report'!$C$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tropical</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'Calc Report'!$B$56:$B$62</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>X1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>X2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>X3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>X4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>X7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calc Report'!$C$56:$C$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.800000000000011</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1521.6000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calc Report'!$D$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Temperate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'Calc Report'!$B$56:$B$62</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>X1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>X2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>X3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>X4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>X7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calc Report'!$D$56:$D$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>123.39999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>199.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1574.8999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calc Report'!$E$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Grass</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'Calc Report'!$B$56:$B$62</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>X1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>X2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>X3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>X4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>X7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calc Report'!$E$56:$E$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>121.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1541.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calc Report'!$F$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Agricultural</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'Calc Report'!$B$56:$B$62</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>X1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>X2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>X3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>X4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>X7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calc Report'!$F$56:$F$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76.399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1525</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calc Report'!$G$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Human</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'Calc Report'!$B$56:$B$62</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>X1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>X2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>X3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>X4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>X7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calc Report'!$G$56:$G$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>149.79999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>102.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>187.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1570.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calc Report'!$H$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tundra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'Calc Report'!$B$56:$B$62</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>X1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>X2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>X3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>X4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>X7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Calc Report'!$H$56:$H$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>149.79999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55.199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1558.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="297222704"/>
+        <c:axId val="297223264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="297222704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Ecosystem Components X</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="-25000"/>
+                  <a:t>i</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>, i=1, 2, ... ,7</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="297223264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="297223264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="89000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="0"/>
+                      <a:lumOff val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="0"/>
+                      <a:lumOff val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="16000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="2700000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Time, Years</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="297222704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2876,6 +4572,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3393,6 +5169,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3956,6 +6764,75 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>61910</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>80964</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4240,8 +7117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B62" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4797,4 +7674,476 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>2.3099999999999999E-2</v>
+      </c>
+      <c r="C1">
+        <v>3.0700000000000002E-2</v>
+      </c>
+      <c r="D1">
+        <v>3.4099999999999998E-2</v>
+      </c>
+      <c r="E1">
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="F1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G1">
+        <v>3.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0.154</v>
+      </c>
+      <c r="C2">
+        <v>0.1024</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0.02</v>
+      </c>
+      <c r="G2">
+        <v>7.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0.70009999999999994</v>
+      </c>
+      <c r="C3">
+        <v>0.92490000000000006</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.15</v>
+      </c>
+      <c r="G3">
+        <v>3.5400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0.154</v>
+      </c>
+      <c r="C4">
+        <v>0.1024</v>
+      </c>
+      <c r="D4">
+        <v>2.2800000000000001E-2</v>
+      </c>
+      <c r="E4">
+        <v>8.6E-3</v>
+      </c>
+      <c r="F4">
+        <v>0.02</v>
+      </c>
+      <c r="G4">
+        <v>4.1999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>6.1600000000000002E-2</v>
+      </c>
+      <c r="C5">
+        <v>8.1900000000000001E-2</v>
+      </c>
+      <c r="D5">
+        <v>6.83E-2</v>
+      </c>
+      <c r="E5">
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="F5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="G5">
+        <v>9.9000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0.40039999999999998</v>
+      </c>
+      <c r="C6">
+        <v>1.74</v>
+      </c>
+      <c r="D6">
+        <v>1.7302</v>
+      </c>
+      <c r="E6">
+        <v>0.38790000000000002</v>
+      </c>
+      <c r="F6">
+        <v>0.3</v>
+      </c>
+      <c r="G6">
+        <v>0.2545</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1.0011000000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.87</v>
+      </c>
+      <c r="D7">
+        <v>1.0813999999999999</v>
+      </c>
+      <c r="E7">
+        <v>0.38790000000000002</v>
+      </c>
+      <c r="F7">
+        <v>0.15</v>
+      </c>
+      <c r="G7">
+        <v>0.1273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <f>B1*10^4</f>
+        <v>231</v>
+      </c>
+      <c r="C11">
+        <f>D1*10^4</f>
+        <v>341</v>
+      </c>
+      <c r="D11">
+        <f>E1*10^4</f>
+        <v>345.00000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:B17" si="0">B2*10^4</f>
+        <v>1540</v>
+      </c>
+      <c r="C12">
+        <f>D2*10^4</f>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f>E2*10^4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>7000.9999999999991</v>
+      </c>
+      <c r="C13">
+        <f>D3*10^4</f>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f>E3*10^4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>1540</v>
+      </c>
+      <c r="C14">
+        <f>D4*10^4</f>
+        <v>228</v>
+      </c>
+      <c r="D14">
+        <f>E4*10^4</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>616</v>
+      </c>
+      <c r="C15">
+        <f>D5*10^4</f>
+        <v>683</v>
+      </c>
+      <c r="D15">
+        <f>E5*10^4</f>
+        <v>345.00000000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>4004</v>
+      </c>
+      <c r="C16">
+        <f>D6*10^4</f>
+        <v>17302</v>
+      </c>
+      <c r="D16">
+        <f>E6*10^4</f>
+        <v>3879</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>10011.000000000002</v>
+      </c>
+      <c r="C17">
+        <f>D7*10^4</f>
+        <v>10814</v>
+      </c>
+      <c r="D17">
+        <f>E7*10^4</f>
+        <v>3879</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="D56">
+        <v>6</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="F56">
+        <v>3</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+      <c r="H56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>30</v>
+      </c>
+      <c r="D57">
+        <v>30</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>30</v>
+      </c>
+      <c r="H57">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>90.800000000000011</v>
+      </c>
+      <c r="D58">
+        <v>180.5</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>149.79999999999998</v>
+      </c>
+      <c r="H58">
+        <v>149.79999999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59">
+        <v>30</v>
+      </c>
+      <c r="D59">
+        <v>30</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
+      </c>
+      <c r="F59">
+        <v>3</v>
+      </c>
+      <c r="G59">
+        <v>30</v>
+      </c>
+      <c r="H59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60">
+        <v>62.4</v>
+      </c>
+      <c r="D60">
+        <v>123.39999999999999</v>
+      </c>
+      <c r="E60">
+        <v>7.4</v>
+      </c>
+      <c r="F60">
+        <v>4.7</v>
+      </c>
+      <c r="G60">
+        <v>102.8</v>
+      </c>
+      <c r="H60">
+        <v>55.199999999999996</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61">
+        <v>64.100000000000009</v>
+      </c>
+      <c r="D61">
+        <v>199.7</v>
+      </c>
+      <c r="E61">
+        <v>121.80000000000001</v>
+      </c>
+      <c r="F61">
+        <v>76.399999999999991</v>
+      </c>
+      <c r="G61">
+        <v>187.5</v>
+      </c>
+      <c r="H61">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62">
+        <v>1521.6000000000001</v>
+      </c>
+      <c r="D62">
+        <v>1574.8999999999999</v>
+      </c>
+      <c r="E62">
+        <v>1541.5</v>
+      </c>
+      <c r="F62">
+        <v>1525</v>
+      </c>
+      <c r="G62">
+        <v>1570.8</v>
+      </c>
+      <c r="H62">
+        <v>1558.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>